<commit_message>
Metadata from data #15
</commit_message>
<xml_diff>
--- a/inst/extdata/2.0.0/metadata/templates/SDTM_METADATA.xlsx
+++ b/inst/extdata/2.0.0/metadata/templates/SDTM_METADATA.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD5E9B6A-97E8-46CB-BAF0-D1D8E58C580D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E45913-D3D9-4F94-9F9F-EF982FBED93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="8"/>
+    <workbookView xWindow="-28920" yWindow="5070" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEFINE_HEADER_METADATA" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">VARIABLE_METADATA!$A$1:$P$160</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -553,14 +553,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -614,7 +608,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -949,7 +943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1017,7 +1011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1026,8 +1020,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
@@ -1041,194 +1035,194 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="H1" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="91" t="s">
+      <c r="I1" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="J1" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="93" t="s">
+      <c r="K1" s="91" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="85"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="83"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
+      <c r="A3" s="92"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
       <c r="K3" s="64"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
       <c r="K4" s="64"/>
     </row>
     <row r="5" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="94"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
       <c r="K5" s="64"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="94"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="94"/>
-      <c r="J6" s="94"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
       <c r="K6" s="64"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="96"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="97"/>
+      <c r="A7" s="94"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="95"/>
       <c r="K7" s="64"/>
     </row>
     <row r="8" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="98"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="96"/>
       <c r="K8" s="42"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="96"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="97"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="95"/>
       <c r="K9" s="64"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="94"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="92"/>
+      <c r="J10" s="92"/>
       <c r="K10" s="64"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
-      <c r="B11" s="94"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
       <c r="K11" s="64"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="96"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="96"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="94"/>
-      <c r="J12" s="97"/>
+      <c r="A12" s="94"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="95"/>
       <c r="K12" s="64"/>
     </row>
     <row r="13" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
       <c r="K13" s="64"/>
     </row>
   </sheetData>
@@ -1239,19 +1233,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P207"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O116" sqref="O116"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="19" style="22" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="21" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" style="21" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" style="22" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" style="21" customWidth="1"/>
@@ -1377,7 +1371,7 @@
       <c r="B5" s="77"/>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
-      <c r="E5" s="80"/>
+      <c r="E5" s="77"/>
       <c r="F5" s="43"/>
       <c r="G5" s="79"/>
       <c r="H5" s="43"/>
@@ -1395,7 +1389,7 @@
       <c r="B6" s="77"/>
       <c r="C6" s="43"/>
       <c r="D6" s="43"/>
-      <c r="E6" s="80"/>
+      <c r="E6" s="77"/>
       <c r="F6" s="43"/>
       <c r="G6" s="79"/>
       <c r="H6" s="43"/>
@@ -1413,8 +1407,8 @@
       <c r="B7" s="77"/>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="81"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="80"/>
       <c r="G7" s="79"/>
       <c r="H7" s="43"/>
       <c r="I7" s="43"/>
@@ -1423,7 +1417,7 @@
       <c r="L7" s="43"/>
       <c r="M7" s="43"/>
       <c r="N7" s="43"/>
-      <c r="O7" s="81"/>
+      <c r="O7" s="80"/>
       <c r="P7" s="42"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1431,8 +1425,8 @@
       <c r="B8" s="77"/>
       <c r="C8" s="43"/>
       <c r="D8" s="43"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="79"/>
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
@@ -1441,7 +1435,7 @@
       <c r="L8" s="43"/>
       <c r="M8" s="43"/>
       <c r="N8" s="43"/>
-      <c r="O8" s="81"/>
+      <c r="O8" s="80"/>
       <c r="P8" s="42"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1449,7 +1443,7 @@
       <c r="B9" s="77"/>
       <c r="C9" s="43"/>
       <c r="D9" s="43"/>
-      <c r="E9" s="80"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="43"/>
       <c r="G9" s="79"/>
       <c r="H9" s="43"/>
@@ -1465,10 +1459,10 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="77"/>
-      <c r="C10" s="81"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="43"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="81"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="79"/>
       <c r="H10" s="43"/>
       <c r="I10" s="43"/>
@@ -1477,16 +1471,16 @@
       <c r="L10" s="43"/>
       <c r="M10" s="43"/>
       <c r="N10" s="43"/>
-      <c r="O10" s="81"/>
+      <c r="O10" s="80"/>
       <c r="P10" s="42"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="43"/>
       <c r="B11" s="77"/>
-      <c r="C11" s="81"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="43"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="81"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="80"/>
       <c r="G11" s="79"/>
       <c r="H11" s="43"/>
       <c r="I11" s="43"/>
@@ -1495,16 +1489,16 @@
       <c r="L11" s="43"/>
       <c r="M11" s="43"/>
       <c r="N11" s="43"/>
-      <c r="O11" s="81"/>
+      <c r="O11" s="80"/>
       <c r="P11" s="42"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="77"/>
-      <c r="C12" s="81"/>
+      <c r="C12" s="80"/>
       <c r="D12" s="43"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="81"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="80"/>
       <c r="G12" s="79"/>
       <c r="H12" s="43"/>
       <c r="I12" s="43"/>
@@ -1513,16 +1507,16 @@
       <c r="L12" s="43"/>
       <c r="M12" s="43"/>
       <c r="N12" s="43"/>
-      <c r="O12" s="81"/>
+      <c r="O12" s="80"/>
       <c r="P12" s="42"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="43"/>
       <c r="B13" s="77"/>
-      <c r="C13" s="81"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="43"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="81"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="80"/>
       <c r="G13" s="79"/>
       <c r="H13" s="43"/>
       <c r="I13" s="43"/>
@@ -1531,16 +1525,16 @@
       <c r="L13" s="43"/>
       <c r="M13" s="43"/>
       <c r="N13" s="43"/>
-      <c r="O13" s="81"/>
+      <c r="O13" s="80"/>
       <c r="P13" s="42"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="77"/>
-      <c r="C14" s="81"/>
+      <c r="C14" s="80"/>
       <c r="D14" s="43"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="81"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="80"/>
       <c r="G14" s="79"/>
       <c r="H14" s="43"/>
       <c r="I14" s="43"/>
@@ -1549,7 +1543,7 @@
       <c r="L14" s="43"/>
       <c r="M14" s="43"/>
       <c r="N14" s="43"/>
-      <c r="O14" s="81"/>
+      <c r="O14" s="80"/>
       <c r="P14" s="42"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1557,7 +1551,7 @@
       <c r="B15" s="77"/>
       <c r="C15" s="43"/>
       <c r="D15" s="43"/>
-      <c r="E15" s="80"/>
+      <c r="E15" s="77"/>
       <c r="F15" s="43"/>
       <c r="G15" s="79"/>
       <c r="H15" s="43"/>
@@ -1573,10 +1567,10 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
       <c r="B16" s="77"/>
-      <c r="C16" s="81"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="43"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="81"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="80"/>
       <c r="G16" s="79"/>
       <c r="H16" s="43"/>
       <c r="I16" s="43"/>
@@ -1591,10 +1585,10 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="43"/>
       <c r="B17" s="77"/>
-      <c r="C17" s="81"/>
+      <c r="C17" s="80"/>
       <c r="D17" s="43"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="81"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="79"/>
       <c r="H17" s="43"/>
       <c r="I17" s="43"/>
@@ -1609,10 +1603,10 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
       <c r="B18" s="77"/>
-      <c r="C18" s="81"/>
+      <c r="C18" s="80"/>
       <c r="D18" s="43"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="81"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="80"/>
       <c r="G18" s="79"/>
       <c r="H18" s="43"/>
       <c r="I18" s="43"/>
@@ -1629,7 +1623,7 @@
       <c r="B19" s="77"/>
       <c r="C19" s="43"/>
       <c r="D19" s="43"/>
-      <c r="E19" s="80"/>
+      <c r="E19" s="77"/>
       <c r="F19" s="43"/>
       <c r="G19" s="79"/>
       <c r="H19" s="43"/>
@@ -1647,7 +1641,7 @@
       <c r="B20" s="77"/>
       <c r="C20" s="43"/>
       <c r="D20" s="43"/>
-      <c r="E20" s="80"/>
+      <c r="E20" s="77"/>
       <c r="F20" s="43"/>
       <c r="G20" s="79"/>
       <c r="H20" s="43"/>
@@ -1665,7 +1659,7 @@
       <c r="B21" s="77"/>
       <c r="C21" s="43"/>
       <c r="D21" s="43"/>
-      <c r="E21" s="82"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="43"/>
       <c r="G21" s="79"/>
       <c r="H21" s="43"/>
@@ -1683,7 +1677,7 @@
       <c r="B22" s="77"/>
       <c r="C22" s="43"/>
       <c r="D22" s="43"/>
-      <c r="E22" s="82"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="43"/>
       <c r="G22" s="79"/>
       <c r="H22" s="43"/>
@@ -1701,7 +1695,7 @@
       <c r="B23" s="77"/>
       <c r="C23" s="43"/>
       <c r="D23" s="43"/>
-      <c r="E23" s="80"/>
+      <c r="E23" s="77"/>
       <c r="F23" s="43"/>
       <c r="G23" s="79"/>
       <c r="H23" s="43"/>
@@ -1717,10 +1711,10 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="43"/>
       <c r="B24" s="77"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="84"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="79"/>
       <c r="H24" s="43"/>
       <c r="I24" s="43"/>
@@ -1729,7 +1723,7 @@
       <c r="L24" s="43"/>
       <c r="M24" s="43"/>
       <c r="N24" s="43"/>
-      <c r="O24" s="84"/>
+      <c r="O24" s="82"/>
       <c r="P24" s="42"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -1773,7 +1767,7 @@
       <c r="B27" s="77"/>
       <c r="C27" s="43"/>
       <c r="D27" s="43"/>
-      <c r="E27" s="80"/>
+      <c r="E27" s="77"/>
       <c r="F27" s="43"/>
       <c r="G27" s="79"/>
       <c r="H27" s="43"/>
@@ -1791,7 +1785,7 @@
       <c r="B28" s="77"/>
       <c r="C28" s="43"/>
       <c r="D28" s="43"/>
-      <c r="E28" s="80"/>
+      <c r="E28" s="77"/>
       <c r="F28" s="43"/>
       <c r="G28" s="79"/>
       <c r="H28" s="43"/>
@@ -1811,7 +1805,7 @@
       <c r="D29" s="43"/>
       <c r="E29" s="77"/>
       <c r="F29" s="43"/>
-      <c r="G29" s="85"/>
+      <c r="G29" s="83"/>
       <c r="H29" s="43"/>
       <c r="I29" s="43"/>
       <c r="J29" s="43"/>
@@ -1915,10 +1909,10 @@
     <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="77"/>
-      <c r="C35" s="81"/>
+      <c r="C35" s="80"/>
       <c r="D35" s="43"/>
       <c r="E35" s="77"/>
-      <c r="F35" s="81"/>
+      <c r="F35" s="80"/>
       <c r="G35" s="79"/>
       <c r="H35" s="43"/>
       <c r="I35" s="43"/>
@@ -1933,10 +1927,10 @@
     <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="43"/>
       <c r="B36" s="77"/>
-      <c r="C36" s="81"/>
+      <c r="C36" s="80"/>
       <c r="D36" s="43"/>
       <c r="E36" s="77"/>
-      <c r="F36" s="81"/>
+      <c r="F36" s="80"/>
       <c r="G36" s="79"/>
       <c r="H36" s="43"/>
       <c r="I36" s="43"/>
@@ -1951,10 +1945,10 @@
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="43"/>
       <c r="B37" s="77"/>
-      <c r="C37" s="81"/>
+      <c r="C37" s="80"/>
       <c r="D37" s="43"/>
       <c r="E37" s="77"/>
-      <c r="F37" s="81"/>
+      <c r="F37" s="80"/>
       <c r="G37" s="79"/>
       <c r="H37" s="43"/>
       <c r="I37" s="43"/>
@@ -1969,10 +1963,10 @@
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="77"/>
-      <c r="C38" s="81"/>
+      <c r="C38" s="80"/>
       <c r="D38" s="43"/>
       <c r="E38" s="77"/>
-      <c r="F38" s="81"/>
+      <c r="F38" s="80"/>
       <c r="G38" s="79"/>
       <c r="H38" s="43"/>
       <c r="I38" s="43"/>
@@ -1987,10 +1981,10 @@
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="43"/>
       <c r="B39" s="77"/>
-      <c r="C39" s="81"/>
+      <c r="C39" s="80"/>
       <c r="D39" s="43"/>
       <c r="E39" s="77"/>
-      <c r="F39" s="81"/>
+      <c r="F39" s="80"/>
       <c r="G39" s="79"/>
       <c r="H39" s="43"/>
       <c r="I39" s="43"/>
@@ -2005,10 +1999,10 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="43"/>
       <c r="B40" s="77"/>
-      <c r="C40" s="81"/>
+      <c r="C40" s="80"/>
       <c r="D40" s="43"/>
       <c r="E40" s="77"/>
-      <c r="F40" s="81"/>
+      <c r="F40" s="80"/>
       <c r="G40" s="79"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
@@ -2170,7 +2164,7 @@
       <c r="C49" s="43"/>
       <c r="D49" s="43"/>
       <c r="E49" s="77"/>
-      <c r="F49" s="81"/>
+      <c r="F49" s="80"/>
       <c r="G49" s="79"/>
       <c r="H49" s="43"/>
       <c r="I49" s="43"/>
@@ -2188,7 +2182,7 @@
       <c r="C50" s="43"/>
       <c r="D50" s="43"/>
       <c r="E50" s="77"/>
-      <c r="F50" s="81"/>
+      <c r="F50" s="80"/>
       <c r="G50" s="79"/>
       <c r="H50" s="43"/>
       <c r="I50" s="43"/>
@@ -2225,7 +2219,7 @@
       <c r="D52" s="43"/>
       <c r="E52" s="77"/>
       <c r="F52" s="43"/>
-      <c r="G52" s="85"/>
+      <c r="G52" s="83"/>
       <c r="H52" s="43"/>
       <c r="I52" s="43"/>
       <c r="J52" s="43"/>
@@ -2277,7 +2271,7 @@
       <c r="B55" s="77"/>
       <c r="C55" s="43"/>
       <c r="D55" s="43"/>
-      <c r="E55" s="80"/>
+      <c r="E55" s="77"/>
       <c r="F55" s="43"/>
       <c r="G55" s="79"/>
       <c r="H55" s="43"/>
@@ -2365,10 +2359,10 @@
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="43"/>
       <c r="B60" s="77"/>
-      <c r="C60" s="83"/>
-      <c r="D60" s="84"/>
-      <c r="E60" s="80"/>
-      <c r="F60" s="84"/>
+      <c r="C60" s="81"/>
+      <c r="D60" s="82"/>
+      <c r="E60" s="77"/>
+      <c r="F60" s="82"/>
       <c r="G60" s="79"/>
       <c r="H60" s="43"/>
       <c r="I60" s="43"/>
@@ -2377,7 +2371,7 @@
       <c r="L60" s="43"/>
       <c r="M60" s="43"/>
       <c r="N60" s="43"/>
-      <c r="O60" s="84"/>
+      <c r="O60" s="82"/>
       <c r="P60" s="42"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -2454,12 +2448,12 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="43"/>
-      <c r="B65" s="86"/>
-      <c r="C65" s="87"/>
+      <c r="B65" s="84"/>
+      <c r="C65" s="85"/>
       <c r="D65" s="43"/>
-      <c r="E65" s="86"/>
-      <c r="F65" s="87"/>
-      <c r="G65" s="85"/>
+      <c r="E65" s="84"/>
+      <c r="F65" s="85"/>
+      <c r="G65" s="83"/>
       <c r="H65" s="43"/>
       <c r="I65" s="43"/>
       <c r="J65" s="43"/>
@@ -2472,11 +2466,11 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="43"/>
-      <c r="B66" s="86"/>
-      <c r="C66" s="87"/>
+      <c r="B66" s="84"/>
+      <c r="C66" s="85"/>
       <c r="D66" s="43"/>
-      <c r="E66" s="86"/>
-      <c r="F66" s="87"/>
+      <c r="E66" s="84"/>
+      <c r="F66" s="85"/>
       <c r="G66" s="79"/>
       <c r="H66" s="43"/>
       <c r="I66" s="43"/>
@@ -2490,11 +2484,11 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="43"/>
-      <c r="B67" s="86"/>
-      <c r="C67" s="87"/>
+      <c r="B67" s="84"/>
+      <c r="C67" s="85"/>
       <c r="D67" s="43"/>
-      <c r="E67" s="86"/>
-      <c r="F67" s="87"/>
+      <c r="E67" s="84"/>
+      <c r="F67" s="85"/>
       <c r="G67" s="79"/>
       <c r="H67" s="43"/>
       <c r="I67" s="43"/>
@@ -2508,11 +2502,11 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="43"/>
-      <c r="B68" s="86"/>
-      <c r="C68" s="87"/>
+      <c r="B68" s="84"/>
+      <c r="C68" s="85"/>
       <c r="D68" s="43"/>
-      <c r="E68" s="86"/>
-      <c r="F68" s="87"/>
+      <c r="E68" s="84"/>
+      <c r="F68" s="85"/>
       <c r="G68" s="79"/>
       <c r="H68" s="43"/>
       <c r="I68" s="43"/>
@@ -2526,11 +2520,11 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="43"/>
-      <c r="B69" s="86"/>
-      <c r="C69" s="87"/>
+      <c r="B69" s="84"/>
+      <c r="C69" s="85"/>
       <c r="D69" s="43"/>
-      <c r="E69" s="86"/>
-      <c r="F69" s="87"/>
+      <c r="E69" s="84"/>
+      <c r="F69" s="85"/>
       <c r="G69" s="79"/>
       <c r="H69" s="43"/>
       <c r="I69" s="43"/>
@@ -2544,11 +2538,11 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="43"/>
-      <c r="B70" s="86"/>
-      <c r="C70" s="87"/>
+      <c r="B70" s="84"/>
+      <c r="C70" s="85"/>
       <c r="D70" s="43"/>
-      <c r="E70" s="86"/>
-      <c r="F70" s="87"/>
+      <c r="E70" s="84"/>
+      <c r="F70" s="85"/>
       <c r="G70" s="79"/>
       <c r="H70" s="43"/>
       <c r="I70" s="43"/>
@@ -2562,11 +2556,11 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="43"/>
-      <c r="B71" s="86"/>
-      <c r="C71" s="87"/>
+      <c r="B71" s="84"/>
+      <c r="C71" s="85"/>
       <c r="D71" s="43"/>
-      <c r="E71" s="86"/>
-      <c r="F71" s="87"/>
+      <c r="E71" s="84"/>
+      <c r="F71" s="85"/>
       <c r="G71" s="79"/>
       <c r="H71" s="43"/>
       <c r="I71" s="43"/>
@@ -2580,11 +2574,11 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="43"/>
-      <c r="B72" s="86"/>
-      <c r="C72" s="87"/>
+      <c r="B72" s="84"/>
+      <c r="C72" s="85"/>
       <c r="D72" s="43"/>
-      <c r="E72" s="86"/>
-      <c r="F72" s="87"/>
+      <c r="E72" s="84"/>
+      <c r="F72" s="85"/>
       <c r="G72" s="79"/>
       <c r="H72" s="43"/>
       <c r="I72" s="43"/>
@@ -2598,11 +2592,11 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="43"/>
-      <c r="B73" s="86"/>
-      <c r="C73" s="87"/>
+      <c r="B73" s="84"/>
+      <c r="C73" s="85"/>
       <c r="D73" s="43"/>
-      <c r="E73" s="86"/>
-      <c r="F73" s="87"/>
+      <c r="E73" s="84"/>
+      <c r="F73" s="85"/>
       <c r="G73" s="79"/>
       <c r="H73" s="43"/>
       <c r="I73" s="43"/>
@@ -2616,11 +2610,11 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="43"/>
-      <c r="B74" s="86"/>
-      <c r="C74" s="87"/>
+      <c r="B74" s="84"/>
+      <c r="C74" s="85"/>
       <c r="D74" s="43"/>
-      <c r="E74" s="86"/>
-      <c r="F74" s="87"/>
+      <c r="E74" s="84"/>
+      <c r="F74" s="85"/>
       <c r="G74" s="79"/>
       <c r="H74" s="43"/>
       <c r="I74" s="43"/>
@@ -2639,7 +2633,7 @@
       <c r="D75" s="43"/>
       <c r="E75" s="77"/>
       <c r="F75" s="43"/>
-      <c r="G75" s="88"/>
+      <c r="G75" s="86"/>
       <c r="H75" s="43"/>
       <c r="I75" s="43"/>
       <c r="J75" s="43"/>
@@ -2691,7 +2685,7 @@
       <c r="B78" s="77"/>
       <c r="C78" s="43"/>
       <c r="D78" s="43"/>
-      <c r="E78" s="80"/>
+      <c r="E78" s="77"/>
       <c r="F78" s="43"/>
       <c r="G78" s="79"/>
       <c r="H78" s="43"/>
@@ -2797,10 +2791,10 @@
     <row r="84" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="43"/>
       <c r="B84" s="77"/>
-      <c r="C84" s="83"/>
+      <c r="C84" s="81"/>
       <c r="D84" s="43"/>
       <c r="E84" s="77"/>
-      <c r="F84" s="84"/>
+      <c r="F84" s="82"/>
       <c r="G84" s="79"/>
       <c r="H84" s="43"/>
       <c r="I84" s="43"/>
@@ -2815,10 +2809,10 @@
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="43"/>
       <c r="B85" s="77"/>
-      <c r="C85" s="83"/>
+      <c r="C85" s="81"/>
       <c r="D85" s="43"/>
       <c r="E85" s="77"/>
-      <c r="F85" s="84"/>
+      <c r="F85" s="82"/>
       <c r="G85" s="79"/>
       <c r="H85" s="43"/>
       <c r="I85" s="43"/>
@@ -2833,10 +2827,10 @@
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="43"/>
       <c r="B86" s="77"/>
-      <c r="C86" s="83"/>
+      <c r="C86" s="81"/>
       <c r="D86" s="43"/>
       <c r="E86" s="77"/>
-      <c r="F86" s="84"/>
+      <c r="F86" s="82"/>
       <c r="G86" s="79"/>
       <c r="H86" s="43"/>
       <c r="I86" s="43"/>
@@ -2851,10 +2845,10 @@
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="43"/>
       <c r="B87" s="77"/>
-      <c r="C87" s="83"/>
+      <c r="C87" s="81"/>
       <c r="D87" s="43"/>
       <c r="E87" s="77"/>
-      <c r="F87" s="84"/>
+      <c r="F87" s="82"/>
       <c r="G87" s="79"/>
       <c r="H87" s="43"/>
       <c r="I87" s="43"/>
@@ -2869,10 +2863,10 @@
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="43"/>
       <c r="B88" s="77"/>
-      <c r="C88" s="83"/>
+      <c r="C88" s="81"/>
       <c r="D88" s="43"/>
       <c r="E88" s="77"/>
-      <c r="F88" s="84"/>
+      <c r="F88" s="82"/>
       <c r="G88" s="79"/>
       <c r="H88" s="43"/>
       <c r="I88" s="43"/>
@@ -2887,10 +2881,10 @@
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="43"/>
       <c r="B89" s="77"/>
-      <c r="C89" s="83"/>
+      <c r="C89" s="81"/>
       <c r="D89" s="43"/>
       <c r="E89" s="77"/>
-      <c r="F89" s="84"/>
+      <c r="F89" s="82"/>
       <c r="G89" s="79"/>
       <c r="H89" s="43"/>
       <c r="I89" s="43"/>
@@ -2905,10 +2899,10 @@
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="43"/>
       <c r="B90" s="77"/>
-      <c r="C90" s="83"/>
+      <c r="C90" s="81"/>
       <c r="D90" s="43"/>
       <c r="E90" s="77"/>
-      <c r="F90" s="84"/>
+      <c r="F90" s="82"/>
       <c r="G90" s="79"/>
       <c r="H90" s="43"/>
       <c r="I90" s="43"/>
@@ -2923,10 +2917,10 @@
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="43"/>
       <c r="B91" s="77"/>
-      <c r="C91" s="83"/>
+      <c r="C91" s="81"/>
       <c r="D91" s="43"/>
       <c r="E91" s="77"/>
-      <c r="F91" s="84"/>
+      <c r="F91" s="82"/>
       <c r="G91" s="79"/>
       <c r="H91" s="43"/>
       <c r="I91" s="43"/>
@@ -2941,10 +2935,10 @@
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="43"/>
       <c r="B92" s="77"/>
-      <c r="C92" s="83"/>
+      <c r="C92" s="81"/>
       <c r="D92" s="43"/>
       <c r="E92" s="77"/>
-      <c r="F92" s="84"/>
+      <c r="F92" s="82"/>
       <c r="G92" s="79"/>
       <c r="H92" s="43"/>
       <c r="I92" s="43"/>
@@ -2995,10 +2989,10 @@
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="43"/>
       <c r="B95" s="77"/>
-      <c r="C95" s="83"/>
-      <c r="D95" s="84"/>
-      <c r="E95" s="80"/>
-      <c r="F95" s="84"/>
+      <c r="C95" s="81"/>
+      <c r="D95" s="82"/>
+      <c r="E95" s="77"/>
+      <c r="F95" s="82"/>
       <c r="G95" s="79"/>
       <c r="H95" s="43"/>
       <c r="I95" s="43"/>
@@ -3007,7 +3001,7 @@
       <c r="L95" s="43"/>
       <c r="M95" s="43"/>
       <c r="N95" s="43"/>
-      <c r="O95" s="84"/>
+      <c r="O95" s="82"/>
       <c r="P95" s="42"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -3016,7 +3010,7 @@
       <c r="C96" s="43"/>
       <c r="D96" s="43"/>
       <c r="E96" s="77"/>
-      <c r="F96" s="84"/>
+      <c r="F96" s="82"/>
       <c r="G96" s="79"/>
       <c r="H96" s="43"/>
       <c r="I96" s="43"/>
@@ -3033,8 +3027,8 @@
       <c r="B97" s="77"/>
       <c r="C97" s="43"/>
       <c r="D97" s="43"/>
-      <c r="E97" s="80"/>
-      <c r="F97" s="84"/>
+      <c r="E97" s="77"/>
+      <c r="F97" s="82"/>
       <c r="G97" s="79"/>
       <c r="H97" s="43"/>
       <c r="I97" s="43"/>
@@ -3049,11 +3043,11 @@
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="43"/>
       <c r="B98" s="77"/>
-      <c r="C98" s="83"/>
-      <c r="D98" s="84"/>
-      <c r="E98" s="80"/>
-      <c r="F98" s="84"/>
-      <c r="G98" s="85"/>
+      <c r="C98" s="81"/>
+      <c r="D98" s="82"/>
+      <c r="E98" s="77"/>
+      <c r="F98" s="82"/>
+      <c r="G98" s="83"/>
       <c r="H98" s="43"/>
       <c r="I98" s="43"/>
       <c r="J98" s="43"/>
@@ -3061,16 +3055,16 @@
       <c r="L98" s="43"/>
       <c r="M98" s="43"/>
       <c r="N98" s="43"/>
-      <c r="O98" s="84"/>
+      <c r="O98" s="82"/>
       <c r="P98" s="42"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="43"/>
       <c r="B99" s="77"/>
-      <c r="C99" s="83"/>
-      <c r="D99" s="84"/>
-      <c r="E99" s="80"/>
-      <c r="F99" s="84"/>
+      <c r="C99" s="81"/>
+      <c r="D99" s="82"/>
+      <c r="E99" s="77"/>
+      <c r="F99" s="82"/>
       <c r="G99" s="79"/>
       <c r="H99" s="43"/>
       <c r="I99" s="43"/>
@@ -3079,16 +3073,16 @@
       <c r="L99" s="43"/>
       <c r="M99" s="43"/>
       <c r="N99" s="43"/>
-      <c r="O99" s="84"/>
+      <c r="O99" s="82"/>
       <c r="P99" s="42"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="43"/>
       <c r="B100" s="77"/>
-      <c r="C100" s="83"/>
-      <c r="D100" s="84"/>
-      <c r="E100" s="80"/>
-      <c r="F100" s="84"/>
+      <c r="C100" s="81"/>
+      <c r="D100" s="82"/>
+      <c r="E100" s="77"/>
+      <c r="F100" s="82"/>
       <c r="G100" s="79"/>
       <c r="H100" s="43"/>
       <c r="I100" s="43"/>
@@ -3097,16 +3091,16 @@
       <c r="L100" s="43"/>
       <c r="M100" s="43"/>
       <c r="N100" s="43"/>
-      <c r="O100" s="84"/>
+      <c r="O100" s="82"/>
       <c r="P100" s="42"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="43"/>
       <c r="B101" s="77"/>
-      <c r="C101" s="83"/>
-      <c r="D101" s="84"/>
-      <c r="E101" s="80"/>
-      <c r="F101" s="84"/>
+      <c r="C101" s="81"/>
+      <c r="D101" s="82"/>
+      <c r="E101" s="77"/>
+      <c r="F101" s="82"/>
       <c r="G101" s="79"/>
       <c r="H101" s="43"/>
       <c r="I101" s="43"/>
@@ -3115,15 +3109,15 @@
       <c r="L101" s="43"/>
       <c r="M101" s="43"/>
       <c r="N101" s="43"/>
-      <c r="O101" s="84"/>
+      <c r="O101" s="82"/>
       <c r="P101" s="42"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="43"/>
       <c r="B102" s="77"/>
-      <c r="C102" s="83"/>
-      <c r="D102" s="84"/>
-      <c r="E102" s="80"/>
+      <c r="C102" s="81"/>
+      <c r="D102" s="82"/>
+      <c r="E102" s="77"/>
       <c r="F102" s="41"/>
       <c r="G102" s="79"/>
       <c r="H102" s="43"/>
@@ -3133,16 +3127,16 @@
       <c r="L102" s="43"/>
       <c r="M102" s="43"/>
       <c r="N102" s="43"/>
-      <c r="O102" s="84"/>
+      <c r="O102" s="82"/>
       <c r="P102" s="42"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="43"/>
       <c r="B103" s="77"/>
-      <c r="C103" s="83"/>
-      <c r="D103" s="84"/>
-      <c r="E103" s="80"/>
-      <c r="F103" s="84"/>
+      <c r="C103" s="81"/>
+      <c r="D103" s="82"/>
+      <c r="E103" s="77"/>
+      <c r="F103" s="82"/>
       <c r="G103" s="79"/>
       <c r="H103" s="43"/>
       <c r="I103" s="43"/>
@@ -3151,16 +3145,16 @@
       <c r="L103" s="43"/>
       <c r="M103" s="43"/>
       <c r="N103" s="43"/>
-      <c r="O103" s="84"/>
+      <c r="O103" s="82"/>
       <c r="P103" s="42"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="43"/>
       <c r="B104" s="77"/>
-      <c r="C104" s="83"/>
-      <c r="D104" s="84"/>
-      <c r="E104" s="80"/>
-      <c r="F104" s="84"/>
+      <c r="C104" s="81"/>
+      <c r="D104" s="82"/>
+      <c r="E104" s="77"/>
+      <c r="F104" s="82"/>
       <c r="G104" s="79"/>
       <c r="H104" s="43"/>
       <c r="I104" s="43"/>
@@ -3169,16 +3163,16 @@
       <c r="L104" s="43"/>
       <c r="M104" s="43"/>
       <c r="N104" s="43"/>
-      <c r="O104" s="84"/>
+      <c r="O104" s="82"/>
       <c r="P104" s="42"/>
     </row>
     <row r="105" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="43"/>
       <c r="B105" s="77"/>
-      <c r="C105" s="83"/>
-      <c r="D105" s="84"/>
-      <c r="E105" s="80"/>
-      <c r="F105" s="84"/>
+      <c r="C105" s="81"/>
+      <c r="D105" s="82"/>
+      <c r="E105" s="77"/>
+      <c r="F105" s="82"/>
       <c r="G105" s="79"/>
       <c r="H105" s="43"/>
       <c r="I105" s="43"/>
@@ -3187,16 +3181,16 @@
       <c r="L105" s="43"/>
       <c r="M105" s="43"/>
       <c r="N105" s="43"/>
-      <c r="O105" s="84"/>
+      <c r="O105" s="82"/>
       <c r="P105" s="42"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="43"/>
       <c r="B106" s="77"/>
-      <c r="C106" s="83"/>
-      <c r="D106" s="84"/>
-      <c r="E106" s="80"/>
-      <c r="F106" s="84"/>
+      <c r="C106" s="81"/>
+      <c r="D106" s="82"/>
+      <c r="E106" s="77"/>
+      <c r="F106" s="82"/>
       <c r="G106" s="79"/>
       <c r="H106" s="43"/>
       <c r="I106" s="43"/>
@@ -3205,16 +3199,16 @@
       <c r="L106" s="43"/>
       <c r="M106" s="43"/>
       <c r="N106" s="43"/>
-      <c r="O106" s="84"/>
+      <c r="O106" s="82"/>
       <c r="P106" s="42"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="43"/>
       <c r="B107" s="77"/>
-      <c r="C107" s="83"/>
-      <c r="D107" s="84"/>
-      <c r="E107" s="80"/>
-      <c r="F107" s="84"/>
+      <c r="C107" s="81"/>
+      <c r="D107" s="82"/>
+      <c r="E107" s="77"/>
+      <c r="F107" s="82"/>
       <c r="G107" s="79"/>
       <c r="H107" s="43"/>
       <c r="I107" s="43"/>
@@ -3223,17 +3217,17 @@
       <c r="L107" s="43"/>
       <c r="M107" s="43"/>
       <c r="N107" s="43"/>
-      <c r="O107" s="84"/>
+      <c r="O107" s="82"/>
       <c r="P107" s="42"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="43"/>
       <c r="B108" s="77"/>
-      <c r="C108" s="83"/>
-      <c r="D108" s="84"/>
-      <c r="E108" s="80"/>
-      <c r="F108" s="84"/>
-      <c r="G108" s="85"/>
+      <c r="C108" s="81"/>
+      <c r="D108" s="82"/>
+      <c r="E108" s="77"/>
+      <c r="F108" s="82"/>
+      <c r="G108" s="83"/>
       <c r="H108" s="43"/>
       <c r="I108" s="43"/>
       <c r="J108" s="43"/>
@@ -3241,16 +3235,16 @@
       <c r="L108" s="43"/>
       <c r="M108" s="43"/>
       <c r="N108" s="43"/>
-      <c r="O108" s="84"/>
+      <c r="O108" s="82"/>
       <c r="P108" s="42"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="43"/>
       <c r="B109" s="77"/>
-      <c r="C109" s="83"/>
-      <c r="D109" s="84"/>
-      <c r="E109" s="80"/>
-      <c r="F109" s="84"/>
+      <c r="C109" s="81"/>
+      <c r="D109" s="82"/>
+      <c r="E109" s="77"/>
+      <c r="F109" s="82"/>
       <c r="G109" s="79"/>
       <c r="H109" s="43"/>
       <c r="I109" s="43"/>
@@ -3259,16 +3253,16 @@
       <c r="L109" s="43"/>
       <c r="M109" s="43"/>
       <c r="N109" s="43"/>
-      <c r="O109" s="84"/>
+      <c r="O109" s="82"/>
       <c r="P109" s="42"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="43"/>
       <c r="B110" s="77"/>
-      <c r="C110" s="83"/>
-      <c r="D110" s="84"/>
-      <c r="E110" s="80"/>
-      <c r="F110" s="84"/>
+      <c r="C110" s="81"/>
+      <c r="D110" s="82"/>
+      <c r="E110" s="77"/>
+      <c r="F110" s="82"/>
       <c r="G110" s="79"/>
       <c r="H110" s="43"/>
       <c r="I110" s="43"/>
@@ -3277,16 +3271,16 @@
       <c r="L110" s="43"/>
       <c r="M110" s="43"/>
       <c r="N110" s="43"/>
-      <c r="O110" s="84"/>
+      <c r="O110" s="82"/>
       <c r="P110" s="42"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="43"/>
       <c r="B111" s="77"/>
-      <c r="C111" s="83"/>
-      <c r="D111" s="84"/>
-      <c r="E111" s="80"/>
-      <c r="F111" s="84"/>
+      <c r="C111" s="81"/>
+      <c r="D111" s="82"/>
+      <c r="E111" s="77"/>
+      <c r="F111" s="82"/>
       <c r="G111" s="79"/>
       <c r="H111" s="43"/>
       <c r="I111" s="43"/>
@@ -3295,16 +3289,16 @@
       <c r="L111" s="43"/>
       <c r="M111" s="43"/>
       <c r="N111" s="43"/>
-      <c r="O111" s="84"/>
+      <c r="O111" s="82"/>
       <c r="P111" s="42"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="43"/>
       <c r="B112" s="77"/>
-      <c r="C112" s="83"/>
-      <c r="D112" s="84"/>
-      <c r="E112" s="80"/>
-      <c r="F112" s="84"/>
+      <c r="C112" s="81"/>
+      <c r="D112" s="82"/>
+      <c r="E112" s="77"/>
+      <c r="F112" s="82"/>
       <c r="G112" s="79"/>
       <c r="H112" s="43"/>
       <c r="I112" s="43"/>
@@ -3313,16 +3307,16 @@
       <c r="L112" s="43"/>
       <c r="M112" s="43"/>
       <c r="N112" s="43"/>
-      <c r="O112" s="84"/>
+      <c r="O112" s="82"/>
       <c r="P112" s="42"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="43"/>
       <c r="B113" s="77"/>
-      <c r="C113" s="83"/>
-      <c r="D113" s="84"/>
-      <c r="E113" s="80"/>
-      <c r="F113" s="84"/>
+      <c r="C113" s="81"/>
+      <c r="D113" s="82"/>
+      <c r="E113" s="77"/>
+      <c r="F113" s="82"/>
       <c r="G113" s="79"/>
       <c r="H113" s="43"/>
       <c r="I113" s="43"/>
@@ -3331,16 +3325,16 @@
       <c r="L113" s="43"/>
       <c r="M113" s="43"/>
       <c r="N113" s="43"/>
-      <c r="O113" s="84"/>
+      <c r="O113" s="82"/>
       <c r="P113" s="42"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="43"/>
       <c r="B114" s="77"/>
-      <c r="C114" s="83"/>
-      <c r="D114" s="84"/>
-      <c r="E114" s="80"/>
-      <c r="F114" s="84"/>
+      <c r="C114" s="81"/>
+      <c r="D114" s="82"/>
+      <c r="E114" s="77"/>
+      <c r="F114" s="82"/>
       <c r="G114" s="79"/>
       <c r="H114" s="43"/>
       <c r="I114" s="43"/>
@@ -3349,17 +3343,17 @@
       <c r="L114" s="43"/>
       <c r="M114" s="43"/>
       <c r="N114" s="43"/>
-      <c r="O114" s="84"/>
+      <c r="O114" s="82"/>
       <c r="P114" s="42"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="43"/>
       <c r="B115" s="77"/>
-      <c r="C115" s="83"/>
-      <c r="D115" s="84"/>
-      <c r="E115" s="80"/>
-      <c r="F115" s="84"/>
-      <c r="G115" s="85"/>
+      <c r="C115" s="81"/>
+      <c r="D115" s="82"/>
+      <c r="E115" s="77"/>
+      <c r="F115" s="82"/>
+      <c r="G115" s="83"/>
       <c r="H115" s="43"/>
       <c r="I115" s="43"/>
       <c r="J115" s="43"/>
@@ -3367,16 +3361,16 @@
       <c r="L115" s="43"/>
       <c r="M115" s="43"/>
       <c r="N115" s="43"/>
-      <c r="O115" s="84"/>
+      <c r="O115" s="82"/>
       <c r="P115" s="42"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="43"/>
       <c r="B116" s="77"/>
-      <c r="C116" s="83"/>
-      <c r="D116" s="84"/>
-      <c r="E116" s="80"/>
-      <c r="F116" s="84"/>
+      <c r="C116" s="81"/>
+      <c r="D116" s="82"/>
+      <c r="E116" s="77"/>
+      <c r="F116" s="82"/>
       <c r="G116" s="79"/>
       <c r="H116" s="43"/>
       <c r="I116" s="43"/>
@@ -3385,15 +3379,15 @@
       <c r="L116" s="43"/>
       <c r="M116" s="43"/>
       <c r="N116" s="43"/>
-      <c r="O116" s="84"/>
+      <c r="O116" s="82"/>
       <c r="P116" s="42"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="43"/>
       <c r="B117" s="77"/>
-      <c r="C117" s="83"/>
-      <c r="D117" s="84"/>
-      <c r="E117" s="80"/>
+      <c r="C117" s="81"/>
+      <c r="D117" s="82"/>
+      <c r="E117" s="77"/>
       <c r="F117" s="41"/>
       <c r="G117" s="79"/>
       <c r="H117" s="43"/>
@@ -3403,16 +3397,16 @@
       <c r="L117" s="43"/>
       <c r="M117" s="43"/>
       <c r="N117" s="43"/>
-      <c r="O117" s="84"/>
+      <c r="O117" s="82"/>
       <c r="P117" s="42"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="43"/>
       <c r="B118" s="77"/>
-      <c r="C118" s="83"/>
-      <c r="D118" s="84"/>
-      <c r="E118" s="80"/>
-      <c r="F118" s="84"/>
+      <c r="C118" s="81"/>
+      <c r="D118" s="82"/>
+      <c r="E118" s="77"/>
+      <c r="F118" s="82"/>
       <c r="G118" s="79"/>
       <c r="H118" s="43"/>
       <c r="I118" s="43"/>
@@ -3421,16 +3415,16 @@
       <c r="L118" s="43"/>
       <c r="M118" s="43"/>
       <c r="N118" s="43"/>
-      <c r="O118" s="84"/>
+      <c r="O118" s="82"/>
       <c r="P118" s="42"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="43"/>
       <c r="B119" s="77"/>
-      <c r="C119" s="83"/>
-      <c r="D119" s="84"/>
-      <c r="E119" s="80"/>
-      <c r="F119" s="84"/>
+      <c r="C119" s="81"/>
+      <c r="D119" s="82"/>
+      <c r="E119" s="77"/>
+      <c r="F119" s="82"/>
       <c r="G119" s="79"/>
       <c r="H119" s="43"/>
       <c r="I119" s="43"/>
@@ -3439,17 +3433,17 @@
       <c r="L119" s="43"/>
       <c r="M119" s="43"/>
       <c r="N119" s="43"/>
-      <c r="O119" s="84"/>
+      <c r="O119" s="82"/>
       <c r="P119" s="42"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="43"/>
       <c r="B120" s="77"/>
-      <c r="C120" s="83"/>
-      <c r="D120" s="84"/>
-      <c r="E120" s="80"/>
-      <c r="F120" s="84"/>
-      <c r="G120" s="85"/>
+      <c r="C120" s="81"/>
+      <c r="D120" s="82"/>
+      <c r="E120" s="77"/>
+      <c r="F120" s="82"/>
+      <c r="G120" s="83"/>
       <c r="H120" s="43"/>
       <c r="I120" s="43"/>
       <c r="J120" s="43"/>
@@ -3457,16 +3451,16 @@
       <c r="L120" s="43"/>
       <c r="M120" s="43"/>
       <c r="N120" s="43"/>
-      <c r="O120" s="84"/>
+      <c r="O120" s="82"/>
       <c r="P120" s="42"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="43"/>
       <c r="B121" s="77"/>
-      <c r="C121" s="83"/>
-      <c r="D121" s="84"/>
-      <c r="E121" s="80"/>
-      <c r="F121" s="84"/>
+      <c r="C121" s="81"/>
+      <c r="D121" s="82"/>
+      <c r="E121" s="77"/>
+      <c r="F121" s="82"/>
       <c r="G121" s="79"/>
       <c r="H121" s="43"/>
       <c r="I121" s="43"/>
@@ -3475,15 +3469,15 @@
       <c r="L121" s="43"/>
       <c r="M121" s="43"/>
       <c r="N121" s="43"/>
-      <c r="O121" s="84"/>
+      <c r="O121" s="82"/>
       <c r="P121" s="42"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="43"/>
       <c r="B122" s="77"/>
-      <c r="C122" s="89"/>
+      <c r="C122" s="87"/>
       <c r="D122" s="41"/>
-      <c r="E122" s="80"/>
+      <c r="E122" s="77"/>
       <c r="F122" s="41"/>
       <c r="G122" s="79"/>
       <c r="H122" s="43"/>
@@ -3499,9 +3493,9 @@
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="43"/>
       <c r="B123" s="77"/>
-      <c r="C123" s="89"/>
+      <c r="C123" s="87"/>
       <c r="D123" s="41"/>
-      <c r="E123" s="80"/>
+      <c r="E123" s="77"/>
       <c r="F123" s="41"/>
       <c r="G123" s="79"/>
       <c r="H123" s="43"/>
@@ -3517,10 +3511,10 @@
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="43"/>
       <c r="B124" s="77"/>
-      <c r="C124" s="89"/>
+      <c r="C124" s="87"/>
       <c r="D124" s="41"/>
-      <c r="E124" s="80"/>
-      <c r="F124" s="84"/>
+      <c r="E124" s="77"/>
+      <c r="F124" s="82"/>
       <c r="G124" s="79"/>
       <c r="H124" s="43"/>
       <c r="I124" s="43"/>
@@ -3535,10 +3529,10 @@
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="43"/>
       <c r="B125" s="77"/>
-      <c r="C125" s="89"/>
+      <c r="C125" s="87"/>
       <c r="D125" s="41"/>
-      <c r="E125" s="80"/>
-      <c r="F125" s="84"/>
+      <c r="E125" s="77"/>
+      <c r="F125" s="82"/>
       <c r="G125" s="79"/>
       <c r="H125" s="43"/>
       <c r="I125" s="43"/>
@@ -3553,9 +3547,9 @@
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="43"/>
       <c r="B126" s="77"/>
-      <c r="C126" s="89"/>
+      <c r="C126" s="87"/>
       <c r="D126" s="41"/>
-      <c r="E126" s="80"/>
+      <c r="E126" s="77"/>
       <c r="F126" s="41"/>
       <c r="G126" s="79"/>
       <c r="H126" s="43"/>
@@ -3571,9 +3565,9 @@
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="43"/>
       <c r="B127" s="77"/>
-      <c r="C127" s="89"/>
+      <c r="C127" s="87"/>
       <c r="D127" s="41"/>
-      <c r="E127" s="80"/>
+      <c r="E127" s="77"/>
       <c r="F127" s="41"/>
       <c r="G127" s="79"/>
       <c r="H127" s="43"/>
@@ -3589,9 +3583,9 @@
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="43"/>
       <c r="B128" s="77"/>
-      <c r="C128" s="89"/>
+      <c r="C128" s="87"/>
       <c r="D128" s="41"/>
-      <c r="E128" s="80"/>
+      <c r="E128" s="77"/>
       <c r="F128" s="41"/>
       <c r="G128" s="79"/>
       <c r="H128" s="43"/>
@@ -3607,11 +3601,11 @@
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="43"/>
       <c r="B129" s="77"/>
-      <c r="C129" s="83"/>
-      <c r="D129" s="84"/>
-      <c r="E129" s="80"/>
-      <c r="F129" s="84"/>
-      <c r="G129" s="85"/>
+      <c r="C129" s="81"/>
+      <c r="D129" s="82"/>
+      <c r="E129" s="77"/>
+      <c r="F129" s="82"/>
+      <c r="G129" s="83"/>
       <c r="H129" s="43"/>
       <c r="I129" s="43"/>
       <c r="J129" s="43"/>
@@ -3619,16 +3613,16 @@
       <c r="L129" s="43"/>
       <c r="M129" s="43"/>
       <c r="N129" s="43"/>
-      <c r="O129" s="84"/>
+      <c r="O129" s="82"/>
       <c r="P129" s="42"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="43"/>
       <c r="B130" s="77"/>
-      <c r="C130" s="83"/>
-      <c r="D130" s="84"/>
-      <c r="E130" s="80"/>
-      <c r="F130" s="84"/>
+      <c r="C130" s="81"/>
+      <c r="D130" s="82"/>
+      <c r="E130" s="77"/>
+      <c r="F130" s="82"/>
       <c r="G130" s="79"/>
       <c r="H130" s="43"/>
       <c r="I130" s="43"/>
@@ -3637,15 +3631,15 @@
       <c r="L130" s="43"/>
       <c r="M130" s="43"/>
       <c r="N130" s="43"/>
-      <c r="O130" s="84"/>
+      <c r="O130" s="82"/>
       <c r="P130" s="42"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="43"/>
       <c r="B131" s="77"/>
-      <c r="C131" s="83"/>
-      <c r="D131" s="84"/>
-      <c r="E131" s="80"/>
+      <c r="C131" s="81"/>
+      <c r="D131" s="82"/>
+      <c r="E131" s="77"/>
       <c r="F131" s="41"/>
       <c r="G131" s="79"/>
       <c r="H131" s="43"/>
@@ -3655,16 +3649,16 @@
       <c r="L131" s="43"/>
       <c r="M131" s="43"/>
       <c r="N131" s="43"/>
-      <c r="O131" s="84"/>
+      <c r="O131" s="82"/>
       <c r="P131" s="42"/>
     </row>
     <row r="132" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="43"/>
       <c r="B132" s="77"/>
-      <c r="C132" s="83"/>
-      <c r="D132" s="84"/>
-      <c r="E132" s="80"/>
-      <c r="F132" s="84"/>
+      <c r="C132" s="81"/>
+      <c r="D132" s="82"/>
+      <c r="E132" s="77"/>
+      <c r="F132" s="82"/>
       <c r="G132" s="79"/>
       <c r="H132" s="43"/>
       <c r="I132" s="43"/>
@@ -3673,15 +3667,15 @@
       <c r="L132" s="43"/>
       <c r="M132" s="43"/>
       <c r="N132" s="43"/>
-      <c r="O132" s="84"/>
+      <c r="O132" s="82"/>
       <c r="P132" s="42"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="43"/>
       <c r="B133" s="77"/>
-      <c r="C133" s="83"/>
-      <c r="D133" s="84"/>
-      <c r="E133" s="80"/>
+      <c r="C133" s="81"/>
+      <c r="D133" s="82"/>
+      <c r="E133" s="77"/>
       <c r="F133" s="41"/>
       <c r="G133" s="79"/>
       <c r="H133" s="43"/>
@@ -3691,16 +3685,16 @@
       <c r="L133" s="43"/>
       <c r="M133" s="43"/>
       <c r="N133" s="43"/>
-      <c r="O133" s="84"/>
+      <c r="O133" s="82"/>
       <c r="P133" s="42"/>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="43"/>
       <c r="B134" s="77"/>
-      <c r="C134" s="83"/>
-      <c r="D134" s="84"/>
-      <c r="E134" s="80"/>
-      <c r="F134" s="84"/>
+      <c r="C134" s="81"/>
+      <c r="D134" s="82"/>
+      <c r="E134" s="77"/>
+      <c r="F134" s="82"/>
       <c r="G134" s="79"/>
       <c r="H134" s="43"/>
       <c r="I134" s="43"/>
@@ -3709,16 +3703,16 @@
       <c r="L134" s="43"/>
       <c r="M134" s="43"/>
       <c r="N134" s="43"/>
-      <c r="O134" s="84"/>
+      <c r="O134" s="82"/>
       <c r="P134" s="42"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="43"/>
       <c r="B135" s="77"/>
-      <c r="C135" s="81"/>
-      <c r="D135" s="84"/>
-      <c r="E135" s="80"/>
-      <c r="F135" s="81"/>
+      <c r="C135" s="80"/>
+      <c r="D135" s="82"/>
+      <c r="E135" s="77"/>
+      <c r="F135" s="80"/>
       <c r="G135" s="79"/>
       <c r="H135" s="43"/>
       <c r="I135" s="43"/>
@@ -3727,16 +3721,16 @@
       <c r="L135" s="43"/>
       <c r="M135" s="43"/>
       <c r="N135" s="43"/>
-      <c r="O135" s="84"/>
+      <c r="O135" s="82"/>
       <c r="P135" s="42"/>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="43"/>
       <c r="B136" s="77"/>
-      <c r="C136" s="81"/>
-      <c r="D136" s="84"/>
-      <c r="E136" s="80"/>
-      <c r="F136" s="81"/>
+      <c r="C136" s="80"/>
+      <c r="D136" s="82"/>
+      <c r="E136" s="77"/>
+      <c r="F136" s="80"/>
       <c r="G136" s="79"/>
       <c r="H136" s="43"/>
       <c r="I136" s="43"/>
@@ -3745,16 +3739,16 @@
       <c r="L136" s="43"/>
       <c r="M136" s="43"/>
       <c r="N136" s="43"/>
-      <c r="O136" s="84"/>
+      <c r="O136" s="82"/>
       <c r="P136" s="42"/>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="43"/>
       <c r="B137" s="77"/>
-      <c r="C137" s="81"/>
-      <c r="D137" s="84"/>
-      <c r="E137" s="80"/>
-      <c r="F137" s="81"/>
+      <c r="C137" s="80"/>
+      <c r="D137" s="82"/>
+      <c r="E137" s="77"/>
+      <c r="F137" s="80"/>
       <c r="G137" s="79"/>
       <c r="H137" s="43"/>
       <c r="I137" s="43"/>
@@ -3763,17 +3757,17 @@
       <c r="L137" s="43"/>
       <c r="M137" s="43"/>
       <c r="N137" s="43"/>
-      <c r="O137" s="84"/>
+      <c r="O137" s="82"/>
       <c r="P137" s="42"/>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="43"/>
       <c r="B138" s="77"/>
-      <c r="C138" s="83"/>
-      <c r="D138" s="84"/>
-      <c r="E138" s="80"/>
-      <c r="F138" s="84"/>
-      <c r="G138" s="85"/>
+      <c r="C138" s="81"/>
+      <c r="D138" s="82"/>
+      <c r="E138" s="77"/>
+      <c r="F138" s="82"/>
+      <c r="G138" s="83"/>
       <c r="H138" s="43"/>
       <c r="I138" s="43"/>
       <c r="J138" s="43"/>
@@ -3781,16 +3775,16 @@
       <c r="L138" s="43"/>
       <c r="M138" s="43"/>
       <c r="N138" s="43"/>
-      <c r="O138" s="84"/>
+      <c r="O138" s="82"/>
       <c r="P138" s="42"/>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="43"/>
       <c r="B139" s="77"/>
-      <c r="C139" s="83"/>
-      <c r="D139" s="84"/>
-      <c r="E139" s="80"/>
-      <c r="F139" s="84"/>
+      <c r="C139" s="81"/>
+      <c r="D139" s="82"/>
+      <c r="E139" s="77"/>
+      <c r="F139" s="82"/>
       <c r="G139" s="79"/>
       <c r="H139" s="43"/>
       <c r="I139" s="43"/>
@@ -3799,16 +3793,16 @@
       <c r="L139" s="43"/>
       <c r="M139" s="43"/>
       <c r="N139" s="43"/>
-      <c r="O139" s="84"/>
+      <c r="O139" s="82"/>
       <c r="P139" s="42"/>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="43"/>
       <c r="B140" s="77"/>
-      <c r="C140" s="83"/>
-      <c r="D140" s="84"/>
-      <c r="E140" s="80"/>
-      <c r="F140" s="84"/>
+      <c r="C140" s="81"/>
+      <c r="D140" s="82"/>
+      <c r="E140" s="77"/>
+      <c r="F140" s="82"/>
       <c r="G140" s="79"/>
       <c r="H140" s="43"/>
       <c r="I140" s="43"/>
@@ -3817,16 +3811,16 @@
       <c r="L140" s="43"/>
       <c r="M140" s="43"/>
       <c r="N140" s="43"/>
-      <c r="O140" s="84"/>
+      <c r="O140" s="82"/>
       <c r="P140" s="42"/>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="43"/>
       <c r="B141" s="77"/>
-      <c r="C141" s="83"/>
-      <c r="D141" s="84"/>
-      <c r="E141" s="80"/>
-      <c r="F141" s="84"/>
+      <c r="C141" s="81"/>
+      <c r="D141" s="82"/>
+      <c r="E141" s="77"/>
+      <c r="F141" s="82"/>
       <c r="G141" s="79"/>
       <c r="H141" s="43"/>
       <c r="I141" s="43"/>
@@ -3835,16 +3829,16 @@
       <c r="L141" s="43"/>
       <c r="M141" s="43"/>
       <c r="N141" s="43"/>
-      <c r="O141" s="84"/>
+      <c r="O141" s="82"/>
       <c r="P141" s="42"/>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="43"/>
       <c r="B142" s="77"/>
-      <c r="C142" s="83"/>
-      <c r="D142" s="84"/>
-      <c r="E142" s="80"/>
-      <c r="F142" s="84"/>
+      <c r="C142" s="81"/>
+      <c r="D142" s="82"/>
+      <c r="E142" s="77"/>
+      <c r="F142" s="82"/>
       <c r="G142" s="79"/>
       <c r="H142" s="43"/>
       <c r="I142" s="43"/>
@@ -3853,16 +3847,16 @@
       <c r="L142" s="43"/>
       <c r="M142" s="43"/>
       <c r="N142" s="43"/>
-      <c r="O142" s="84"/>
+      <c r="O142" s="82"/>
       <c r="P142" s="42"/>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="43"/>
       <c r="B143" s="77"/>
-      <c r="C143" s="83"/>
-      <c r="D143" s="84"/>
-      <c r="E143" s="80"/>
-      <c r="F143" s="84"/>
+      <c r="C143" s="81"/>
+      <c r="D143" s="82"/>
+      <c r="E143" s="77"/>
+      <c r="F143" s="82"/>
       <c r="G143" s="79"/>
       <c r="H143" s="43"/>
       <c r="I143" s="43"/>
@@ -3871,16 +3865,16 @@
       <c r="L143" s="43"/>
       <c r="M143" s="43"/>
       <c r="N143" s="43"/>
-      <c r="O143" s="84"/>
+      <c r="O143" s="82"/>
       <c r="P143" s="42"/>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="43"/>
       <c r="B144" s="77"/>
-      <c r="C144" s="83"/>
-      <c r="D144" s="84"/>
-      <c r="E144" s="80"/>
-      <c r="F144" s="84"/>
+      <c r="C144" s="81"/>
+      <c r="D144" s="82"/>
+      <c r="E144" s="77"/>
+      <c r="F144" s="82"/>
       <c r="G144" s="79"/>
       <c r="H144" s="43"/>
       <c r="I144" s="43"/>
@@ -3889,16 +3883,16 @@
       <c r="L144" s="43"/>
       <c r="M144" s="43"/>
       <c r="N144" s="43"/>
-      <c r="O144" s="84"/>
+      <c r="O144" s="82"/>
       <c r="P144" s="42"/>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="43"/>
       <c r="B145" s="77"/>
-      <c r="C145" s="83"/>
-      <c r="D145" s="84"/>
-      <c r="E145" s="80"/>
-      <c r="F145" s="84"/>
+      <c r="C145" s="81"/>
+      <c r="D145" s="82"/>
+      <c r="E145" s="77"/>
+      <c r="F145" s="82"/>
       <c r="G145" s="79"/>
       <c r="H145" s="43"/>
       <c r="I145" s="43"/>
@@ -3907,7 +3901,7 @@
       <c r="L145" s="43"/>
       <c r="M145" s="43"/>
       <c r="N145" s="43"/>
-      <c r="O145" s="84"/>
+      <c r="O145" s="82"/>
       <c r="P145" s="42"/>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
@@ -3917,7 +3911,7 @@
       <c r="D146" s="43"/>
       <c r="E146" s="77"/>
       <c r="F146" s="43"/>
-      <c r="G146" s="85"/>
+      <c r="G146" s="83"/>
       <c r="H146" s="43"/>
       <c r="I146" s="43"/>
       <c r="J146" s="43"/>
@@ -3969,7 +3963,7 @@
       <c r="B149" s="77"/>
       <c r="C149" s="43"/>
       <c r="D149" s="43"/>
-      <c r="E149" s="80"/>
+      <c r="E149" s="77"/>
       <c r="F149" s="43"/>
       <c r="G149" s="79"/>
       <c r="H149" s="43"/>
@@ -4042,7 +4036,7 @@
       <c r="C153" s="43"/>
       <c r="D153" s="43"/>
       <c r="E153" s="77"/>
-      <c r="F153" s="84"/>
+      <c r="F153" s="82"/>
       <c r="G153" s="79"/>
       <c r="H153" s="43"/>
       <c r="I153" s="43"/>
@@ -4075,10 +4069,10 @@
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="43"/>
       <c r="B155" s="77"/>
-      <c r="C155" s="83"/>
-      <c r="D155" s="84"/>
-      <c r="E155" s="80"/>
-      <c r="F155" s="84"/>
+      <c r="C155" s="81"/>
+      <c r="D155" s="82"/>
+      <c r="E155" s="77"/>
+      <c r="F155" s="82"/>
       <c r="G155" s="79"/>
       <c r="H155" s="43"/>
       <c r="I155" s="43"/>
@@ -4087,7 +4081,7 @@
       <c r="L155" s="43"/>
       <c r="M155" s="43"/>
       <c r="N155" s="43"/>
-      <c r="O155" s="84"/>
+      <c r="O155" s="82"/>
       <c r="P155" s="42"/>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
@@ -4129,10 +4123,10 @@
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="43"/>
       <c r="B158" s="77"/>
-      <c r="C158" s="89"/>
+      <c r="C158" s="87"/>
       <c r="D158" s="43"/>
       <c r="E158" s="77"/>
-      <c r="F158" s="84"/>
+      <c r="F158" s="82"/>
       <c r="G158" s="79"/>
       <c r="H158" s="43"/>
       <c r="I158" s="43"/>
@@ -4150,7 +4144,7 @@
       <c r="C159" s="43"/>
       <c r="D159" s="43"/>
       <c r="E159" s="77"/>
-      <c r="F159" s="84"/>
+      <c r="F159" s="82"/>
       <c r="G159" s="79"/>
       <c r="H159" s="43"/>
       <c r="I159" s="43"/>
@@ -4167,8 +4161,8 @@
       <c r="B160" s="77"/>
       <c r="C160" s="43"/>
       <c r="D160" s="43"/>
-      <c r="E160" s="80"/>
-      <c r="F160" s="84"/>
+      <c r="E160" s="77"/>
+      <c r="F160" s="82"/>
       <c r="G160" s="79"/>
       <c r="H160" s="43"/>
       <c r="I160" s="43"/>
@@ -4182,10 +4176,10 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" s="48"/>
-      <c r="B161" s="90"/>
+      <c r="B161" s="88"/>
       <c r="C161" s="48"/>
       <c r="D161" s="48"/>
-      <c r="E161" s="90"/>
+      <c r="E161" s="88"/>
       <c r="F161" s="48"/>
       <c r="G161" s="79"/>
       <c r="H161" s="48"/>
@@ -4200,10 +4194,10 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" s="48"/>
-      <c r="B162" s="90"/>
+      <c r="B162" s="88"/>
       <c r="C162" s="48"/>
       <c r="D162" s="48"/>
-      <c r="E162" s="90"/>
+      <c r="E162" s="88"/>
       <c r="F162" s="48"/>
       <c r="G162" s="79"/>
       <c r="H162" s="48"/>
@@ -4218,10 +4212,10 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" s="48"/>
-      <c r="B163" s="90"/>
+      <c r="B163" s="88"/>
       <c r="C163" s="48"/>
       <c r="D163" s="48"/>
-      <c r="E163" s="90"/>
+      <c r="E163" s="88"/>
       <c r="F163" s="48"/>
       <c r="G163" s="79"/>
       <c r="H163" s="48"/>
@@ -4236,10 +4230,10 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" s="48"/>
-      <c r="B164" s="90"/>
+      <c r="B164" s="88"/>
       <c r="C164" s="48"/>
       <c r="D164" s="48"/>
-      <c r="E164" s="90"/>
+      <c r="E164" s="88"/>
       <c r="F164" s="48"/>
       <c r="G164" s="79"/>
       <c r="H164" s="48"/>
@@ -4254,10 +4248,10 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="48"/>
-      <c r="B165" s="90"/>
+      <c r="B165" s="88"/>
       <c r="C165" s="48"/>
       <c r="D165" s="48"/>
-      <c r="E165" s="90"/>
+      <c r="E165" s="88"/>
       <c r="F165" s="48"/>
       <c r="G165" s="79"/>
       <c r="H165" s="48"/>
@@ -4272,10 +4266,10 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" s="48"/>
-      <c r="B166" s="90"/>
+      <c r="B166" s="88"/>
       <c r="C166" s="48"/>
       <c r="D166" s="48"/>
-      <c r="E166" s="90"/>
+      <c r="E166" s="88"/>
       <c r="F166" s="48"/>
       <c r="G166" s="79"/>
       <c r="H166" s="48"/>
@@ -4290,10 +4284,10 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" s="48"/>
-      <c r="B167" s="90"/>
+      <c r="B167" s="88"/>
       <c r="C167" s="48"/>
       <c r="D167" s="48"/>
-      <c r="E167" s="90"/>
+      <c r="E167" s="88"/>
       <c r="F167" s="48"/>
       <c r="G167" s="79"/>
       <c r="H167" s="48"/>
@@ -4308,10 +4302,10 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" s="48"/>
-      <c r="B168" s="90"/>
+      <c r="B168" s="88"/>
       <c r="C168" s="48"/>
       <c r="D168" s="48"/>
-      <c r="E168" s="90"/>
+      <c r="E168" s="88"/>
       <c r="F168" s="48"/>
       <c r="G168" s="79"/>
       <c r="H168" s="48"/>
@@ -4326,10 +4320,10 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" s="48"/>
-      <c r="B169" s="90"/>
+      <c r="B169" s="88"/>
       <c r="C169" s="48"/>
       <c r="D169" s="48"/>
-      <c r="E169" s="90"/>
+      <c r="E169" s="88"/>
       <c r="F169" s="48"/>
       <c r="G169" s="79"/>
       <c r="H169" s="48"/>
@@ -4344,10 +4338,10 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" s="48"/>
-      <c r="B170" s="90"/>
+      <c r="B170" s="88"/>
       <c r="C170" s="48"/>
       <c r="D170" s="48"/>
-      <c r="E170" s="90"/>
+      <c r="E170" s="88"/>
       <c r="F170" s="48"/>
       <c r="G170" s="79"/>
       <c r="H170" s="48"/>
@@ -4362,10 +4356,10 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" s="48"/>
-      <c r="B171" s="90"/>
+      <c r="B171" s="88"/>
       <c r="C171" s="48"/>
       <c r="D171" s="48"/>
-      <c r="E171" s="90"/>
+      <c r="E171" s="88"/>
       <c r="F171" s="48"/>
       <c r="G171" s="79"/>
       <c r="H171" s="48"/>
@@ -4380,10 +4374,10 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" s="48"/>
-      <c r="B172" s="90"/>
+      <c r="B172" s="88"/>
       <c r="C172" s="48"/>
       <c r="D172" s="48"/>
-      <c r="E172" s="90"/>
+      <c r="E172" s="88"/>
       <c r="F172" s="48"/>
       <c r="G172" s="79"/>
       <c r="H172" s="48"/>
@@ -4398,10 +4392,10 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" s="48"/>
-      <c r="B173" s="90"/>
+      <c r="B173" s="88"/>
       <c r="C173" s="48"/>
       <c r="D173" s="48"/>
-      <c r="E173" s="90"/>
+      <c r="E173" s="88"/>
       <c r="F173" s="48"/>
       <c r="G173" s="79"/>
       <c r="H173" s="48"/>
@@ -4416,10 +4410,10 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="48"/>
-      <c r="B174" s="90"/>
+      <c r="B174" s="88"/>
       <c r="C174" s="48"/>
       <c r="D174" s="48"/>
-      <c r="E174" s="90"/>
+      <c r="E174" s="88"/>
       <c r="F174" s="48"/>
       <c r="G174" s="79"/>
       <c r="H174" s="48"/>
@@ -4434,10 +4428,10 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" s="48"/>
-      <c r="B175" s="90"/>
+      <c r="B175" s="88"/>
       <c r="C175" s="48"/>
       <c r="D175" s="48"/>
-      <c r="E175" s="90"/>
+      <c r="E175" s="88"/>
       <c r="F175" s="48"/>
       <c r="G175" s="79"/>
       <c r="H175" s="48"/>
@@ -4452,10 +4446,10 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" s="48"/>
-      <c r="B176" s="90"/>
+      <c r="B176" s="88"/>
       <c r="C176" s="48"/>
       <c r="D176" s="48"/>
-      <c r="E176" s="90"/>
+      <c r="E176" s="88"/>
       <c r="F176" s="48"/>
       <c r="G176" s="79"/>
       <c r="H176" s="48"/>
@@ -4470,10 +4464,10 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" s="48"/>
-      <c r="B177" s="90"/>
+      <c r="B177" s="88"/>
       <c r="C177" s="48"/>
       <c r="D177" s="48"/>
-      <c r="E177" s="90"/>
+      <c r="E177" s="88"/>
       <c r="F177" s="48"/>
       <c r="G177" s="79"/>
       <c r="H177" s="48"/>
@@ -4488,10 +4482,10 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" s="48"/>
-      <c r="B178" s="90"/>
+      <c r="B178" s="88"/>
       <c r="C178" s="48"/>
       <c r="D178" s="48"/>
-      <c r="E178" s="90"/>
+      <c r="E178" s="88"/>
       <c r="F178" s="48"/>
       <c r="G178" s="79"/>
       <c r="H178" s="48"/>
@@ -4506,10 +4500,10 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" s="48"/>
-      <c r="B179" s="90"/>
+      <c r="B179" s="88"/>
       <c r="C179" s="48"/>
       <c r="D179" s="48"/>
-      <c r="E179" s="90"/>
+      <c r="E179" s="88"/>
       <c r="F179" s="48"/>
       <c r="G179" s="79"/>
       <c r="H179" s="48"/>
@@ -4524,10 +4518,10 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" s="48"/>
-      <c r="B180" s="90"/>
+      <c r="B180" s="88"/>
       <c r="C180" s="48"/>
       <c r="D180" s="48"/>
-      <c r="E180" s="90"/>
+      <c r="E180" s="88"/>
       <c r="F180" s="48"/>
       <c r="G180" s="79"/>
       <c r="H180" s="48"/>
@@ -4542,10 +4536,10 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" s="48"/>
-      <c r="B181" s="90"/>
+      <c r="B181" s="88"/>
       <c r="C181" s="48"/>
       <c r="D181" s="48"/>
-      <c r="E181" s="90"/>
+      <c r="E181" s="88"/>
       <c r="F181" s="48"/>
       <c r="G181" s="79"/>
       <c r="H181" s="48"/>
@@ -4560,10 +4554,10 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" s="48"/>
-      <c r="B182" s="90"/>
+      <c r="B182" s="88"/>
       <c r="C182" s="48"/>
       <c r="D182" s="48"/>
-      <c r="E182" s="90"/>
+      <c r="E182" s="88"/>
       <c r="F182" s="48"/>
       <c r="G182" s="79"/>
       <c r="H182" s="48"/>
@@ -4578,10 +4572,10 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" s="48"/>
-      <c r="B183" s="90"/>
+      <c r="B183" s="88"/>
       <c r="C183" s="48"/>
       <c r="D183" s="48"/>
-      <c r="E183" s="90"/>
+      <c r="E183" s="88"/>
       <c r="F183" s="48"/>
       <c r="G183" s="79"/>
       <c r="H183" s="48"/>
@@ -4596,10 +4590,10 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" s="48"/>
-      <c r="B184" s="90"/>
+      <c r="B184" s="88"/>
       <c r="C184" s="48"/>
       <c r="D184" s="48"/>
-      <c r="E184" s="90"/>
+      <c r="E184" s="88"/>
       <c r="F184" s="48"/>
       <c r="G184" s="79"/>
       <c r="H184" s="48"/>
@@ -4614,10 +4608,10 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" s="48"/>
-      <c r="B185" s="90"/>
+      <c r="B185" s="88"/>
       <c r="C185" s="48"/>
       <c r="D185" s="48"/>
-      <c r="E185" s="90"/>
+      <c r="E185" s="88"/>
       <c r="F185" s="48"/>
       <c r="G185" s="79"/>
       <c r="H185" s="48"/>
@@ -4632,10 +4626,10 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" s="48"/>
-      <c r="B186" s="90"/>
+      <c r="B186" s="88"/>
       <c r="C186" s="48"/>
       <c r="D186" s="48"/>
-      <c r="E186" s="90"/>
+      <c r="E186" s="88"/>
       <c r="F186" s="48"/>
       <c r="G186" s="79"/>
       <c r="H186" s="48"/>
@@ -4650,10 +4644,10 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" s="48"/>
-      <c r="B187" s="90"/>
+      <c r="B187" s="88"/>
       <c r="C187" s="48"/>
       <c r="D187" s="48"/>
-      <c r="E187" s="90"/>
+      <c r="E187" s="88"/>
       <c r="F187" s="48"/>
       <c r="G187" s="79"/>
       <c r="H187" s="48"/>
@@ -4668,10 +4662,10 @@
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" s="48"/>
-      <c r="B188" s="90"/>
+      <c r="B188" s="88"/>
       <c r="C188" s="48"/>
       <c r="D188" s="48"/>
-      <c r="E188" s="90"/>
+      <c r="E188" s="88"/>
       <c r="F188" s="48"/>
       <c r="G188" s="79"/>
       <c r="H188" s="48"/>
@@ -4686,10 +4680,10 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" s="48"/>
-      <c r="B189" s="90"/>
+      <c r="B189" s="88"/>
       <c r="C189" s="48"/>
       <c r="D189" s="48"/>
-      <c r="E189" s="90"/>
+      <c r="E189" s="88"/>
       <c r="F189" s="48"/>
       <c r="G189" s="79"/>
       <c r="H189" s="48"/>
@@ -4704,10 +4698,10 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" s="48"/>
-      <c r="B190" s="90"/>
+      <c r="B190" s="88"/>
       <c r="C190" s="48"/>
       <c r="D190" s="48"/>
-      <c r="E190" s="90"/>
+      <c r="E190" s="88"/>
       <c r="F190" s="48"/>
       <c r="G190" s="79"/>
       <c r="H190" s="48"/>
@@ -4722,10 +4716,10 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" s="48"/>
-      <c r="B191" s="90"/>
+      <c r="B191" s="88"/>
       <c r="C191" s="48"/>
       <c r="D191" s="48"/>
-      <c r="E191" s="90"/>
+      <c r="E191" s="88"/>
       <c r="F191" s="48"/>
       <c r="G191" s="79"/>
       <c r="H191" s="48"/>
@@ -4740,10 +4734,10 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" s="48"/>
-      <c r="B192" s="90"/>
+      <c r="B192" s="88"/>
       <c r="C192" s="48"/>
       <c r="D192" s="48"/>
-      <c r="E192" s="90"/>
+      <c r="E192" s="88"/>
       <c r="F192" s="48"/>
       <c r="G192" s="79"/>
       <c r="H192" s="48"/>
@@ -4758,10 +4752,10 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" s="48"/>
-      <c r="B193" s="90"/>
+      <c r="B193" s="88"/>
       <c r="C193" s="48"/>
       <c r="D193" s="48"/>
-      <c r="E193" s="90"/>
+      <c r="E193" s="88"/>
       <c r="F193" s="48"/>
       <c r="G193" s="79"/>
       <c r="H193" s="48"/>
@@ -4776,10 +4770,10 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" s="48"/>
-      <c r="B194" s="90"/>
+      <c r="B194" s="88"/>
       <c r="C194" s="48"/>
       <c r="D194" s="48"/>
-      <c r="E194" s="90"/>
+      <c r="E194" s="88"/>
       <c r="F194" s="48"/>
       <c r="G194" s="79"/>
       <c r="H194" s="48"/>
@@ -4794,10 +4788,10 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" s="48"/>
-      <c r="B195" s="90"/>
+      <c r="B195" s="88"/>
       <c r="C195" s="48"/>
       <c r="D195" s="48"/>
-      <c r="E195" s="90"/>
+      <c r="E195" s="88"/>
       <c r="F195" s="48"/>
       <c r="G195" s="79"/>
       <c r="H195" s="48"/>
@@ -4812,10 +4806,10 @@
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" s="48"/>
-      <c r="B196" s="90"/>
+      <c r="B196" s="88"/>
       <c r="C196" s="48"/>
       <c r="D196" s="48"/>
-      <c r="E196" s="90"/>
+      <c r="E196" s="88"/>
       <c r="F196" s="48"/>
       <c r="G196" s="79"/>
       <c r="H196" s="48"/>
@@ -4830,10 +4824,10 @@
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" s="48"/>
-      <c r="B197" s="90"/>
+      <c r="B197" s="88"/>
       <c r="C197" s="48"/>
       <c r="D197" s="48"/>
-      <c r="E197" s="90"/>
+      <c r="E197" s="88"/>
       <c r="F197" s="48"/>
       <c r="G197" s="79"/>
       <c r="H197" s="48"/>
@@ -4848,10 +4842,10 @@
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" s="48"/>
-      <c r="B198" s="90"/>
+      <c r="B198" s="88"/>
       <c r="C198" s="48"/>
       <c r="D198" s="48"/>
-      <c r="E198" s="90"/>
+      <c r="E198" s="88"/>
       <c r="F198" s="48"/>
       <c r="G198" s="79"/>
       <c r="H198" s="48"/>
@@ -4866,10 +4860,10 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" s="48"/>
-      <c r="B199" s="90"/>
+      <c r="B199" s="88"/>
       <c r="C199" s="48"/>
       <c r="D199" s="48"/>
-      <c r="E199" s="90"/>
+      <c r="E199" s="88"/>
       <c r="F199" s="48"/>
       <c r="G199" s="79"/>
       <c r="H199" s="48"/>
@@ -4884,10 +4878,10 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" s="48"/>
-      <c r="B200" s="90"/>
+      <c r="B200" s="88"/>
       <c r="C200" s="48"/>
       <c r="D200" s="48"/>
-      <c r="E200" s="90"/>
+      <c r="E200" s="88"/>
       <c r="F200" s="48"/>
       <c r="G200" s="79"/>
       <c r="H200" s="48"/>
@@ -4902,10 +4896,10 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" s="48"/>
-      <c r="B201" s="90"/>
+      <c r="B201" s="88"/>
       <c r="C201" s="48"/>
       <c r="D201" s="48"/>
-      <c r="E201" s="90"/>
+      <c r="E201" s="88"/>
       <c r="F201" s="48"/>
       <c r="G201" s="79"/>
       <c r="H201" s="48"/>
@@ -4920,10 +4914,10 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" s="48"/>
-      <c r="B202" s="90"/>
+      <c r="B202" s="88"/>
       <c r="C202" s="48"/>
       <c r="D202" s="48"/>
-      <c r="E202" s="90"/>
+      <c r="E202" s="88"/>
       <c r="F202" s="48"/>
       <c r="G202" s="79"/>
       <c r="H202" s="48"/>
@@ -4938,10 +4932,10 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" s="48"/>
-      <c r="B203" s="90"/>
+      <c r="B203" s="88"/>
       <c r="C203" s="48"/>
       <c r="D203" s="48"/>
-      <c r="E203" s="90"/>
+      <c r="E203" s="88"/>
       <c r="F203" s="48"/>
       <c r="G203" s="79"/>
       <c r="H203" s="48"/>
@@ -4956,10 +4950,10 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" s="48"/>
-      <c r="B204" s="90"/>
+      <c r="B204" s="88"/>
       <c r="C204" s="48"/>
       <c r="D204" s="48"/>
-      <c r="E204" s="90"/>
+      <c r="E204" s="88"/>
       <c r="F204" s="48"/>
       <c r="G204" s="79"/>
       <c r="H204" s="48"/>
@@ -4974,10 +4968,10 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" s="48"/>
-      <c r="B205" s="90"/>
+      <c r="B205" s="88"/>
       <c r="C205" s="48"/>
       <c r="D205" s="48"/>
-      <c r="E205" s="90"/>
+      <c r="E205" s="88"/>
       <c r="F205" s="48"/>
       <c r="G205" s="79"/>
       <c r="H205" s="48"/>
@@ -4992,10 +4986,10 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" s="48"/>
-      <c r="B206" s="90"/>
+      <c r="B206" s="88"/>
       <c r="C206" s="48"/>
       <c r="D206" s="48"/>
-      <c r="E206" s="90"/>
+      <c r="E206" s="88"/>
       <c r="F206" s="48"/>
       <c r="G206" s="79"/>
       <c r="H206" s="48"/>
@@ -5010,10 +5004,10 @@
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" s="48"/>
-      <c r="B207" s="90"/>
+      <c r="B207" s="88"/>
       <c r="C207" s="48"/>
       <c r="D207" s="48"/>
-      <c r="E207" s="90"/>
+      <c r="E207" s="88"/>
       <c r="F207" s="48"/>
       <c r="G207" s="79"/>
       <c r="H207" s="48"/>
@@ -5027,14 +5021,14 @@
       <c r="P207" s="42"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P160"/>
+  <autoFilter ref="A1:P160" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -5535,7 +5529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5785,7 +5779,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N160"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8407,7 +8401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8490,7 +8484,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8526,10 +8520,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>